<commit_message>
Fix missing map keys for "OTHER" bank account mappings
Updated "OTHER" mappings for bankAccountType and usWireInternationalData to reference the correct custom entity fields. This ensures
</commit_message>
<xml_diff>
--- a/TechDoc/map.xlsx
+++ b/TechDoc/map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoranroncevic/WebstormProjects/creednz/TechDoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9838C3F1-7296-704E-962E-173BF2F82B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509EEFD1-68F1-4748-95C5-1E92BD440C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{D9C87440-CC64-554B-9733-CC1A40CFC103}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16320" xr2:uid="{D9C87440-CC64-554B-9733-CC1A40CFC103}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
   <si>
     <t>iCA</t>
   </si>
@@ -101,20 +101,38 @@
     <t>ABA</t>
   </si>
   <si>
-    <t xml:space="preserve">custentity_vendorbranchbankircid </t>
-  </si>
-  <si>
     <t>any</t>
   </si>
   <si>
     <t>OTHER</t>
+  </si>
+  <si>
+    <t>paymentCategory</t>
+  </si>
+  <si>
+    <t>paymentFormat</t>
+  </si>
+  <si>
+    <t>custentity_paymentformat</t>
+  </si>
+  <si>
+    <t>bankName</t>
+  </si>
+  <si>
+    <t>custentity_bankname</t>
+  </si>
+  <si>
+    <t>usWireInternationalData</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +156,18 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -168,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -176,6 +206,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6448111E-6D7B-8647-A747-F3BDC4F7146A}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="93" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="93" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,15 +553,18 @@
     <col min="1" max="1" width="29.33203125" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
-    <col min="9" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" customWidth="1"/>
+    <col min="13" max="14" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -540,7 +575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -550,29 +585,41 @@
       <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -582,24 +629,36 @@
       <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -609,23 +668,35 @@
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -633,36 +704,66 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>2</v>
+      <c r="J6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>